<commit_message>
fix templates, limpieza imports y creación de utils
</commit_message>
<xml_diff>
--- a/flask/app/static/files/exportaciones/solicitudes_entrantes.xlsx
+++ b/flask/app/static/files/exportaciones/solicitudes_entrantes.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Solicitudes por revisar" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Solicitudes por revisar" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -70,92 +70,24 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -448,7 +380,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,14 +388,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="15"/>
-    <col customWidth="1" max="2" min="2" width="13"/>
-    <col customWidth="1" max="3" min="3" width="19"/>
-    <col customWidth="1" max="4" min="4" width="22"/>
-    <col customWidth="1" max="5" min="5" width="20"/>
-    <col customWidth="1" max="6" min="6" width="16"/>
-    <col customWidth="1" max="7" min="7" width="19"/>
-    <col customWidth="1" max="8" min="8" width="19"/>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="13" customWidth="1" min="2" max="2"/>
+    <col width="19" customWidth="1" min="3" max="3"/>
+    <col width="22" customWidth="1" min="4" max="4"/>
+    <col width="30" customWidth="1" min="5" max="5"/>
+    <col width="16" customWidth="1" min="6" max="6"/>
+    <col width="19" customWidth="1" min="7" max="7"/>
+    <col width="27" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -510,261 +442,321 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>276</v>
+        <v>251</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>867</v>
+        <v>750</v>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>199543172</t>
+          <t>19988806K</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>Cristóbal Flores</t>
+          <t>Sebastián Toro</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>Consola Sony PS5</t>
+          <t>Baterias 9V Bateria Bateria</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>SONYPS</t>
+          <t>M01P04BAT1-3</t>
         </is>
       </c>
       <c r="G2" s="3" t="n">
-        <v>44112.6247337963</v>
-      </c>
-      <c r="H2" s="2" t="n"/>
+        <v>44134.03646990741</v>
+      </c>
+      <c r="H2" s="2" t="inlineStr">
+        <is>
+          <t>BASES DE DATOS</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>270</v>
+        <v>251</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>849</v>
+        <v>751</v>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
-          <t>199029932</t>
+          <t>19988806K</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>Ariel Gomez Cifuentes</t>
+          <t>Sebastián Toro</t>
         </is>
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>Drone Parrot Bebop 2</t>
+          <t>Baterias 9V Bateria Bateria</t>
         </is>
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>ABC432</t>
+          <t>M01P04BAT1-3</t>
         </is>
       </c>
       <c r="G3" s="3" t="n">
-        <v>44112.0656712963</v>
-      </c>
-      <c r="H3" s="2" t="n"/>
+        <v>44134.03646990741</v>
+      </c>
+      <c r="H3" s="2" t="inlineStr">
+        <is>
+          <t>EVALUACIÓN DE PROYECTOS TIC</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>834</v>
+        <v>752</v>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>188639089</t>
+          <t>19988806K</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>Lino Cisternas</t>
+          <t>Sebastián Toro</t>
         </is>
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>Consola Sony PS5</t>
+          <t>Baterias 9V Bateria Bateria</t>
         </is>
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>SONYPS</t>
+          <t>M01P04BAT1-3</t>
         </is>
       </c>
       <c r="G4" s="3" t="n">
-        <v>44111.03188657408</v>
-      </c>
-      <c r="H4" s="2" t="n"/>
+        <v>44134.03646990741</v>
+      </c>
+      <c r="H4" s="2" t="inlineStr">
+        <is>
+          <t>EVALUACIÓN DE PROYECTOS TIC</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>831</v>
+        <v>747</v>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>188639089</t>
+          <t>19988806K</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>Lino Cisternas</t>
+          <t>Sebastián Toro</t>
         </is>
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>Consola Sony PS5</t>
+          <t xml:space="preserve">Grapas  </t>
         </is>
       </c>
       <c r="F5" s="2" t="inlineStr">
         <is>
-          <t>SONYPS</t>
+          <t>M01P01GP01-1</t>
         </is>
       </c>
       <c r="G5" s="3" t="n">
-        <v>44111.03188657408</v>
-      </c>
-      <c r="H5" s="2" t="n"/>
+        <v>44134.02997685185</v>
+      </c>
+      <c r="H5" s="2" t="inlineStr">
+        <is>
+          <t>DESARROLLO WEB Y MÓVIL</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>833</v>
+        <v>748</v>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>188639089</t>
+          <t>19988806K</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>Lino Cisternas</t>
+          <t>Sebastián Toro</t>
         </is>
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>Consola Sony PS5</t>
+          <t xml:space="preserve">Grapas  </t>
         </is>
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
-          <t>SONYPS</t>
+          <t>M01P01GP01-1</t>
         </is>
       </c>
       <c r="G6" s="3" t="n">
-        <v>44111.03188657408</v>
-      </c>
-      <c r="H6" s="2" t="n"/>
+        <v>44134.02997685185</v>
+      </c>
+      <c r="H6" s="2" t="inlineStr">
+        <is>
+          <t>DESARROLLO WEB Y MÓVIL</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>830</v>
+        <v>745</v>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>188639089</t>
+          <t>19988806K</t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>Lino Cisternas</t>
+          <t>Sebastián Toro</t>
         </is>
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>Consola Sony PS5</t>
+          <t xml:space="preserve">Pycom  </t>
         </is>
       </c>
       <c r="F7" s="2" t="inlineStr">
         <is>
-          <t>SONYPS</t>
+          <t>M01P01PCM1-7</t>
         </is>
       </c>
       <c r="G7" s="3" t="n">
-        <v>44111.03188657408</v>
-      </c>
-      <c r="H7" s="2" t="n"/>
+        <v>44134.02997685185</v>
+      </c>
+      <c r="H7" s="2" t="inlineStr">
+        <is>
+          <t>ASEGURAMIENTO DE LA CALIDAD</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>832</v>
+        <v>746</v>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>188639089</t>
+          <t>19988806K</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>Lino Cisternas</t>
+          <t>Sebastián Toro</t>
         </is>
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>Consola Sony PS5</t>
+          <t xml:space="preserve">Grapas  </t>
         </is>
       </c>
       <c r="F8" s="2" t="inlineStr">
         <is>
-          <t>SONYPS</t>
+          <t>M01P01GP01-1</t>
         </is>
       </c>
       <c r="G8" s="3" t="n">
-        <v>44111.03188657408</v>
-      </c>
-      <c r="H8" s="2" t="n"/>
+        <v>44134.02997685185</v>
+      </c>
+      <c r="H8" s="2" t="inlineStr">
+        <is>
+          <t>DESARROLLO WEB Y MÓVIL</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>264</v>
+        <v>247</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>828</v>
+        <v>738</v>
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>188639089</t>
+          <t>19988806K</t>
         </is>
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>Lino Cisternas</t>
+          <t>Sebastián Toro</t>
         </is>
       </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
-          <t>Consola Sony PS5</t>
+          <t>Drone Toshibas Raspberry Pi B+</t>
         </is>
       </c>
       <c r="F9" s="2" t="inlineStr">
         <is>
-          <t>SONYPS</t>
+          <t>LIC01P04</t>
         </is>
       </c>
       <c r="G9" s="3" t="n">
-        <v>44111.02668981482</v>
+        <v>44132.88994212963</v>
       </c>
       <c r="H9" s="2" t="n"/>
     </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>247</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>739</v>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>19988806K</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>Sebastián Toro</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>Drone Toshibas Raspberry Pi B+</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>LIC01P04</t>
+        </is>
+      </c>
+      <c r="G10" s="3" t="n">
+        <v>44132.88994212963</v>
+      </c>
+      <c r="H10" s="2" t="n"/>
+    </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>